<commit_message>
adds zero for NA in 2014
</commit_message>
<xml_diff>
--- a/Mariana_Crow_MARK.xlsx
+++ b/Mariana_Crow_MARK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coldwater/TeachLearn/TeamAga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE2C40-F5D4-6843-BCBB-63A8AC2CA09A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0550CE77-EB78-8844-97CB-C807D3C8CD79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23000" windowHeight="13480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,11 +183,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -313,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,9 +595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -720,6 +722,9 @@
       <c r="R2" s="1">
         <v>0</v>
       </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -776,6 +781,9 @@
       <c r="R3" s="1">
         <v>1</v>
       </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -832,6 +840,9 @@
       <c r="R4" s="1">
         <v>0</v>
       </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -888,6 +899,9 @@
       <c r="R5" s="1">
         <v>0</v>
       </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -944,6 +958,9 @@
       <c r="R6" s="1">
         <v>0</v>
       </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1000,6 +1017,9 @@
       <c r="R7" s="1">
         <v>0</v>
       </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1056,6 +1076,9 @@
       <c r="R8" s="1">
         <v>0</v>
       </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1112,6 +1135,9 @@
       <c r="R9" s="1">
         <v>0</v>
       </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1168,6 +1194,9 @@
       <c r="R10" s="1">
         <v>0</v>
       </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1224,6 +1253,9 @@
       <c r="R11" s="1">
         <v>0</v>
       </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1280,6 +1312,9 @@
       <c r="R12" s="1">
         <v>0</v>
       </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1336,6 +1371,9 @@
       <c r="R13" s="1">
         <v>0</v>
       </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1392,6 +1430,9 @@
       <c r="R14" s="1">
         <v>0</v>
       </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1448,6 +1489,9 @@
       <c r="R15" s="1">
         <v>0</v>
       </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1504,8 +1548,11 @@
       <c r="R16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>76448101</v>
       </c>
@@ -1560,8 +1607,11 @@
       <c r="R17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>76448103</v>
       </c>
@@ -1616,8 +1666,11 @@
       <c r="R18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>76448104</v>
       </c>
@@ -1672,8 +1725,11 @@
       <c r="R19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>76448105</v>
       </c>
@@ -1728,8 +1784,11 @@
       <c r="R20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>76448106</v>
       </c>
@@ -1784,8 +1843,11 @@
       <c r="R21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>76448107</v>
       </c>
@@ -1840,8 +1902,11 @@
       <c r="R22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>76448108</v>
       </c>
@@ -1896,8 +1961,11 @@
       <c r="R23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>76448109</v>
       </c>
@@ -1952,8 +2020,11 @@
       <c r="R24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>76448110</v>
       </c>
@@ -2008,8 +2079,11 @@
       <c r="R25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>76448111</v>
       </c>
@@ -2064,8 +2138,11 @@
       <c r="R26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>76448112</v>
       </c>
@@ -2120,8 +2197,11 @@
       <c r="R27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>76448113</v>
       </c>
@@ -2176,8 +2256,11 @@
       <c r="R28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>76448114</v>
       </c>
@@ -2232,8 +2315,11 @@
       <c r="R29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>76448115</v>
       </c>
@@ -2288,8 +2374,11 @@
       <c r="R30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>76448116</v>
       </c>
@@ -2344,8 +2433,11 @@
       <c r="R31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>76448117</v>
       </c>
@@ -2400,8 +2492,11 @@
       <c r="R32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>76448118</v>
       </c>
@@ -2456,8 +2551,11 @@
       <c r="R33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>76448119</v>
       </c>
@@ -2512,8 +2610,11 @@
       <c r="R34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>76448120</v>
       </c>
@@ -2568,8 +2669,11 @@
       <c r="R35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>76448121</v>
       </c>
@@ -2624,8 +2728,11 @@
       <c r="R36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>76448122</v>
       </c>
@@ -2680,8 +2787,11 @@
       <c r="R37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>76448123</v>
       </c>
@@ -2736,8 +2846,11 @@
       <c r="R38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>76448124</v>
       </c>
@@ -2792,8 +2905,11 @@
       <c r="R39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>76448125</v>
       </c>
@@ -2848,8 +2964,11 @@
       <c r="R40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>76448126</v>
       </c>
@@ -2904,8 +3023,11 @@
       <c r="R41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>76448127</v>
       </c>
@@ -2960,8 +3082,11 @@
       <c r="R42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>76448128</v>
       </c>
@@ -3016,8 +3141,11 @@
       <c r="R43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>76448129</v>
       </c>
@@ -3072,8 +3200,11 @@
       <c r="R44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>76448132</v>
       </c>
@@ -3128,8 +3259,11 @@
       <c r="R45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>76448134</v>
       </c>
@@ -3184,8 +3318,11 @@
       <c r="R46" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>76448135</v>
       </c>
@@ -3240,8 +3377,11 @@
       <c r="R47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>76448136</v>
       </c>
@@ -3296,8 +3436,11 @@
       <c r="R48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>76448137</v>
       </c>
@@ -3352,8 +3495,11 @@
       <c r="R49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>76448138</v>
       </c>
@@ -3408,8 +3554,11 @@
       <c r="R50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>76448139</v>
       </c>
@@ -3464,8 +3613,11 @@
       <c r="R51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>76448140</v>
       </c>
@@ -3520,8 +3672,11 @@
       <c r="R52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>76448141</v>
       </c>
@@ -3576,8 +3731,11 @@
       <c r="R53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>76448142</v>
       </c>
@@ -3632,8 +3790,11 @@
       <c r="R54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>76448143</v>
       </c>
@@ -3688,8 +3849,11 @@
       <c r="R55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>76448144</v>
       </c>
@@ -3744,8 +3908,11 @@
       <c r="R56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>76448145</v>
       </c>
@@ -3800,8 +3967,11 @@
       <c r="R57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>76448146</v>
       </c>
@@ -3856,8 +4026,11 @@
       <c r="R58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>76448147</v>
       </c>
@@ -3912,8 +4085,11 @@
       <c r="R59" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>76448148</v>
       </c>
@@ -3968,8 +4144,11 @@
       <c r="R60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>76469311</v>
       </c>
@@ -4024,8 +4203,11 @@
       <c r="R61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>76469323</v>
       </c>
@@ -4080,8 +4262,11 @@
       <c r="R62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>76469397</v>
       </c>
@@ -4136,8 +4321,11 @@
       <c r="R63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>76469398</v>
       </c>
@@ -4192,8 +4380,11 @@
       <c r="R64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>76469399</v>
       </c>
@@ -4248,8 +4439,11 @@
       <c r="R65" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>76469400</v>
       </c>
@@ -4304,8 +4498,11 @@
       <c r="R66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>84477201</v>
       </c>
@@ -4360,8 +4557,11 @@
       <c r="R67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>84477202</v>
       </c>
@@ -4416,8 +4616,11 @@
       <c r="R68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>84477203</v>
       </c>
@@ -4472,8 +4675,11 @@
       <c r="R69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>84477204</v>
       </c>
@@ -4528,8 +4734,11 @@
       <c r="R70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>84477205</v>
       </c>
@@ -4584,8 +4793,11 @@
       <c r="R71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>84477206</v>
       </c>
@@ -4640,8 +4852,11 @@
       <c r="R72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>84477208</v>
       </c>
@@ -4696,8 +4911,11 @@
       <c r="R73" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>84477209</v>
       </c>
@@ -4752,8 +4970,11 @@
       <c r="R74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>84477210</v>
       </c>
@@ -4808,8 +5029,11 @@
       <c r="R75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>84477211</v>
       </c>
@@ -4864,8 +5088,11 @@
       <c r="R76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>84477212</v>
       </c>
@@ -4920,8 +5147,11 @@
       <c r="R77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>84477213</v>
       </c>
@@ -4976,8 +5206,11 @@
       <c r="R78" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>84477214</v>
       </c>
@@ -5032,8 +5265,11 @@
       <c r="R79" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>84477215</v>
       </c>
@@ -5088,8 +5324,11 @@
       <c r="R80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>84477216</v>
       </c>
@@ -5144,8 +5383,11 @@
       <c r="R81" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>84477217</v>
       </c>
@@ -5200,8 +5442,11 @@
       <c r="R82" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>84477218</v>
       </c>
@@ -5256,8 +5501,11 @@
       <c r="R83" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>84477219</v>
       </c>
@@ -5312,8 +5560,11 @@
       <c r="R84" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84477220</v>
       </c>
@@ -5368,8 +5619,11 @@
       <c r="R85" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84477221</v>
       </c>
@@ -5424,8 +5678,11 @@
       <c r="R86" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>84477222</v>
       </c>
@@ -5480,8 +5737,11 @@
       <c r="R87" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84477223</v>
       </c>
@@ -5536,8 +5796,11 @@
       <c r="R88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>84477224</v>
       </c>
@@ -5592,8 +5855,11 @@
       <c r="R89" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>84477225</v>
       </c>
@@ -5648,8 +5914,11 @@
       <c r="R90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>84477228</v>
       </c>
@@ -5704,8 +5973,11 @@
       <c r="R91" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>84477230</v>
       </c>
@@ -5760,8 +6032,11 @@
       <c r="R92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>84477232</v>
       </c>
@@ -5816,8 +6091,11 @@
       <c r="R93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>84477233</v>
       </c>
@@ -5872,8 +6150,11 @@
       <c r="R94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>84477234</v>
       </c>
@@ -5928,8 +6209,11 @@
       <c r="R95" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>84477235</v>
       </c>
@@ -5984,8 +6268,11 @@
       <c r="R96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>84477236</v>
       </c>
@@ -6040,8 +6327,11 @@
       <c r="R97" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>84477237</v>
       </c>
@@ -6096,8 +6386,11 @@
       <c r="R98" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>84477238</v>
       </c>
@@ -6152,8 +6445,11 @@
       <c r="R99" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>84477239</v>
       </c>
@@ -6208,8 +6504,11 @@
       <c r="R100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>84477240</v>
       </c>
@@ -6264,8 +6563,11 @@
       <c r="R101" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>84477242</v>
       </c>
@@ -6320,8 +6622,11 @@
       <c r="R102" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>84477243</v>
       </c>
@@ -6376,8 +6681,11 @@
       <c r="R103" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>84477244</v>
       </c>
@@ -6432,8 +6740,11 @@
       <c r="R104" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>84477246</v>
       </c>
@@ -6488,8 +6799,11 @@
       <c r="R105" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>84477247</v>
       </c>
@@ -6544,8 +6858,11 @@
       <c r="R106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>84477249</v>
       </c>
@@ -6600,8 +6917,11 @@
       <c r="R107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>84477250</v>
       </c>
@@ -6656,8 +6976,11 @@
       <c r="R108" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>84477253</v>
       </c>
@@ -6712,8 +7035,11 @@
       <c r="R109" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>84477255</v>
       </c>
@@ -6768,8 +7094,11 @@
       <c r="R110" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>99403002</v>
       </c>
@@ -6824,8 +7153,11 @@
       <c r="R111" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>99403004</v>
       </c>
@@ -6878,6 +7210,9 @@
         <v>1</v>
       </c>
       <c r="R112" s="1">
+        <v>0</v>
+      </c>
+      <c r="S112" s="1">
         <v>0</v>
       </c>
     </row>
@@ -6936,6 +7271,9 @@
       <c r="R113" s="1">
         <v>0</v>
       </c>
+      <c r="S113" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
@@ -6992,6 +7330,9 @@
       <c r="R114" s="1">
         <v>0</v>
       </c>
+      <c r="S114" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
@@ -7048,6 +7389,9 @@
       <c r="R115" s="1">
         <v>1</v>
       </c>
+      <c r="S115" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
@@ -7104,6 +7448,9 @@
       <c r="R116" s="1">
         <v>0</v>
       </c>
+      <c r="S116" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
@@ -7160,6 +7507,9 @@
       <c r="R117" s="1">
         <v>0</v>
       </c>
+      <c r="S117" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
@@ -7216,6 +7566,9 @@
       <c r="R118" s="1">
         <v>0</v>
       </c>
+      <c r="S118" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
@@ -7272,6 +7625,9 @@
       <c r="R119" s="1">
         <v>1</v>
       </c>
+      <c r="S119" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
@@ -7328,6 +7684,9 @@
       <c r="R120" s="1">
         <v>1</v>
       </c>
+      <c r="S120" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
@@ -7384,6 +7743,9 @@
       <c r="R121" s="1">
         <v>1</v>
       </c>
+      <c r="S121" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
@@ -7440,6 +7802,9 @@
       <c r="R122" s="1">
         <v>1</v>
       </c>
+      <c r="S122" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
@@ -7496,6 +7861,9 @@
       <c r="R123" s="1">
         <v>1</v>
       </c>
+      <c r="S123" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
@@ -7552,6 +7920,9 @@
       <c r="R124" s="1">
         <v>1</v>
       </c>
+      <c r="S124" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
@@ -7608,6 +7979,9 @@
       <c r="R125" s="1">
         <v>1</v>
       </c>
+      <c r="S125" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
@@ -7664,6 +8038,9 @@
       <c r="R126" s="1">
         <v>0</v>
       </c>
+      <c r="S126" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
@@ -7718,6 +8095,9 @@
         <v>0</v>
       </c>
       <c r="R127" s="1">
+        <v>0</v>
+      </c>
+      <c r="S127" s="1">
         <v>0</v>
       </c>
     </row>
@@ -18542,71 +18922,71 @@
     </row>
     <row r="158" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C158" s="1">
-        <f>SUM(C2:C157)</f>
+        <f t="shared" ref="C158:S158" si="0">SUM(C2:C157)</f>
         <v>34</v>
       </c>
       <c r="D158" s="1">
-        <f>SUM(D2:D157)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E158" s="1">
-        <f>SUM(E2:E157)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F158" s="1">
-        <f>SUM(F2:F157)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G158" s="1">
-        <f>SUM(G2:G157)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H158" s="1">
-        <f>SUM(H2:H157)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I158" s="1">
-        <f>SUM(I2:I157)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J158" s="1">
-        <f>SUM(J2:J157)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K158" s="1">
-        <f>SUM(K2:K157)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L158" s="1">
-        <f>SUM(L2:L157)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="M158" s="1">
-        <f>SUM(M2:M157)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="N158" s="1">
-        <f>SUM(N2:N157)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="O158" s="1">
-        <f>SUM(O2:O157)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="P158" s="1">
-        <f>SUM(P2:P157)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="Q158" s="1">
-        <f>SUM(Q2:Q157)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="R158" s="1">
-        <f>SUM(R2:R157)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="S158" s="1">
-        <f>SUM(S2:S157)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>

</xml_diff>